<commit_message>
Added and seperated analysis for Person B
</commit_message>
<xml_diff>
--- a/Person_B_and_trucks/on_trucks/Processed_Stand_Alone/10_245-70R19.xlsx
+++ b/Person_B_and_trucks/on_trucks/Processed_Stand_Alone/10_245-70R19.xlsx
@@ -21,109 +21,109 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="57">
   <si>
-    <t>Signal_Value_88</t>
-  </si>
-  <si>
-    <t>Signal_Value_89</t>
-  </si>
-  <si>
-    <t>Signal_Value_90</t>
-  </si>
-  <si>
-    <t>Signal_Value_91</t>
-  </si>
-  <si>
-    <t>Signal_Value_92</t>
-  </si>
-  <si>
-    <t>Signal_Value_93</t>
-  </si>
-  <si>
-    <t>Signal_Value_94</t>
-  </si>
-  <si>
-    <t>Signal_Value_95</t>
-  </si>
-  <si>
-    <t>Signal_Value_96</t>
-  </si>
-  <si>
-    <t>Signal_Value_97</t>
-  </si>
-  <si>
-    <t>Signal_Value_98</t>
-  </si>
-  <si>
-    <t>Signal_Value_99</t>
-  </si>
-  <si>
-    <t>Signal_Value_100</t>
-  </si>
-  <si>
-    <t>Signal_Value_101</t>
-  </si>
-  <si>
-    <t>Signal_Value_102</t>
-  </si>
-  <si>
-    <t>Signal_Value_103</t>
-  </si>
-  <si>
-    <t>Signal_Value_104</t>
-  </si>
-  <si>
-    <t>Signal_Value_105</t>
-  </si>
-  <si>
-    <t>Signal_Value_106</t>
-  </si>
-  <si>
-    <t>Signal_Value_107</t>
-  </si>
-  <si>
-    <t>Signal_Value_108</t>
-  </si>
-  <si>
-    <t>Signal_Value_109</t>
-  </si>
-  <si>
-    <t>Signal_Value_110</t>
-  </si>
-  <si>
-    <t>Signal_Value_111</t>
-  </si>
-  <si>
-    <t>Signal_Value_112</t>
-  </si>
-  <si>
-    <t>Signal_Value_113</t>
-  </si>
-  <si>
-    <t>Signal_Value_114</t>
-  </si>
-  <si>
-    <t>Signal_Value_115</t>
-  </si>
-  <si>
-    <t>Signal_Value_116</t>
-  </si>
-  <si>
-    <t>Signal_Value_117</t>
-  </si>
-  <si>
-    <t>Signal_Value_118</t>
-  </si>
-  <si>
-    <t>Signal_Value_119</t>
-  </si>
-  <si>
-    <t>Signal_Value_120</t>
-  </si>
-  <si>
-    <t>Signal_Value_121</t>
-  </si>
-  <si>
-    <t>Signal_Value_122</t>
+    <t>Signal_Value_49</t>
+  </si>
+  <si>
+    <t>Signal_Value_50</t>
+  </si>
+  <si>
+    <t>Signal_Value_51</t>
+  </si>
+  <si>
+    <t>Signal_Value_52</t>
+  </si>
+  <si>
+    <t>Signal_Value_53</t>
+  </si>
+  <si>
+    <t>Signal_Value_54</t>
+  </si>
+  <si>
+    <t>Signal_Value_55</t>
+  </si>
+  <si>
+    <t>Signal_Value_56</t>
+  </si>
+  <si>
+    <t>Signal_Value_57</t>
+  </si>
+  <si>
+    <t>Signal_Value_58</t>
+  </si>
+  <si>
+    <t>Signal_Value_59</t>
+  </si>
+  <si>
+    <t>Signal_Value_60</t>
+  </si>
+  <si>
+    <t>Signal_Value_61</t>
+  </si>
+  <si>
+    <t>Signal_Value_62</t>
+  </si>
+  <si>
+    <t>Signal_Value_63</t>
+  </si>
+  <si>
+    <t>Signal_Value_64</t>
+  </si>
+  <si>
+    <t>Signal_Value_65</t>
+  </si>
+  <si>
+    <t>Signal_Value_66</t>
+  </si>
+  <si>
+    <t>Signal_Value_67</t>
+  </si>
+  <si>
+    <t>Signal_Value_68</t>
+  </si>
+  <si>
+    <t>Signal_Value_69</t>
+  </si>
+  <si>
+    <t>Signal_Value_70</t>
+  </si>
+  <si>
+    <t>Signal_Value_71</t>
+  </si>
+  <si>
+    <t>Signal_Value_72</t>
+  </si>
+  <si>
+    <t>Signal_Value_73</t>
+  </si>
+  <si>
+    <t>Signal_Value_74</t>
+  </si>
+  <si>
+    <t>Signal_Value_75</t>
+  </si>
+  <si>
+    <t>Signal_Value_76</t>
+  </si>
+  <si>
+    <t>Signal_Value_77</t>
+  </si>
+  <si>
+    <t>Signal_Value_78</t>
+  </si>
+  <si>
+    <t>Signal_Value_79</t>
+  </si>
+  <si>
+    <t>Signal_Value_80</t>
+  </si>
+  <si>
+    <t>Signal_Value_81</t>
+  </si>
+  <si>
+    <t>Signal_Value_82</t>
+  </si>
+  <si>
+    <t>Signal_Value_83</t>
   </si>
   <si>
     <t>Segment_ID</t>
@@ -674,73 +674,73 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>0.002056664043484111</v>
       </c>
       <c r="E2">
-        <v>0.1883562720413256</v>
+        <v>0.129334167665091</v>
       </c>
       <c r="F2">
-        <v>0.02510516389178956</v>
+        <v>0.02072565488618068</v>
       </c>
       <c r="G2">
-        <v>0.2806140951908258</v>
+        <v>0.2755030635257049</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>0.06612825498102003</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>0.02041544467279583</v>
       </c>
       <c r="J2">
-        <v>0.01799627644658349</v>
+        <v>0</v>
       </c>
       <c r="K2">
-        <v>0.09188788860966107</v>
+        <v>0</v>
       </c>
       <c r="L2">
         <v>0</v>
       </c>
       <c r="M2">
-        <v>0.01772962084126473</v>
+        <v>0.2405682824292601</v>
       </c>
       <c r="N2">
-        <v>0.08651575188835429</v>
+        <v>0.04740479292504285</v>
       </c>
       <c r="O2">
-        <v>0.007515628400145689</v>
+        <v>0</v>
       </c>
       <c r="P2">
-        <v>0</v>
+        <v>0.05875091417251681</v>
       </c>
       <c r="Q2">
-        <v>0</v>
+        <v>0.009822985698967083</v>
       </c>
       <c r="R2">
-        <v>0.0679215628021367</v>
+        <v>0.01983851680862085</v>
       </c>
       <c r="S2">
-        <v>0.009354707817189264</v>
+        <v>0.01339703983617692</v>
       </c>
       <c r="T2">
-        <v>0.009409078027060314</v>
+        <v>0</v>
       </c>
       <c r="U2">
-        <v>0.06249699576466432</v>
+        <v>0</v>
       </c>
       <c r="V2">
         <v>0</v>
       </c>
       <c r="W2">
-        <v>0.0009130098233818617</v>
+        <v>0.02581443201604547</v>
       </c>
       <c r="X2">
-        <v>0.08538596395270243</v>
+        <v>0.02574345689215807</v>
       </c>
       <c r="Y2">
-        <v>0.01451133998321967</v>
+        <v>0.01037491380084151</v>
       </c>
       <c r="Z2">
-        <v>0.02045269134469629</v>
+        <v>0</v>
       </c>
       <c r="AA2">
         <v>0</v>
@@ -767,10 +767,10 @@
         <v>0</v>
       </c>
       <c r="AI2">
-        <v>0</v>
+        <v>0.03412141564609376</v>
       </c>
       <c r="AJ2">
-        <v>0.0138339531749992</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:36">
@@ -787,70 +787,70 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0.2810718858277978</v>
+        <v>0.1714552967088327</v>
       </c>
       <c r="F3">
-        <v>0.09570109906500639</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>0.3081852082731207</v>
+        <v>0.1268710911921427</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>0.1378342289241996</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>0.06823849261464773</v>
       </c>
       <c r="J3">
-        <v>0.0043345091647187</v>
+        <v>0</v>
       </c>
       <c r="K3">
-        <v>0.1147149655833565</v>
+        <v>0</v>
       </c>
       <c r="L3">
-        <v>0.00793617876372193</v>
+        <v>0</v>
       </c>
       <c r="M3">
-        <v>0.02655650898660795</v>
+        <v>0.153850546015204</v>
       </c>
       <c r="N3">
-        <v>0.01184477026260017</v>
+        <v>0.03204187273025869</v>
       </c>
       <c r="O3">
         <v>0</v>
       </c>
       <c r="P3">
-        <v>0</v>
+        <v>0.08062121855260755</v>
       </c>
       <c r="Q3">
-        <v>0.002125668525927968</v>
+        <v>0</v>
       </c>
       <c r="R3">
-        <v>0.007929201533682935</v>
+        <v>0.06660888750725841</v>
       </c>
       <c r="S3">
-        <v>0.02547915724157416</v>
+        <v>0</v>
       </c>
       <c r="T3">
         <v>0</v>
       </c>
       <c r="U3">
-        <v>0.01472853565955751</v>
+        <v>0.008471117633059612</v>
       </c>
       <c r="V3">
         <v>0</v>
       </c>
       <c r="W3">
-        <v>0</v>
+        <v>0.007658505086714576</v>
       </c>
       <c r="X3">
-        <v>0.06350268928220477</v>
+        <v>0.02478325568067999</v>
       </c>
       <c r="Y3">
-        <v>0</v>
+        <v>0.02018285149994988</v>
       </c>
       <c r="Z3">
-        <v>0.005367150936926981</v>
+        <v>0</v>
       </c>
       <c r="AA3">
         <v>0</v>
@@ -865,7 +865,7 @@
         <v>0</v>
       </c>
       <c r="AE3">
-        <v>0</v>
+        <v>0.01160321557743421</v>
       </c>
       <c r="AF3">
         <v>0</v>
@@ -874,13 +874,13 @@
         <v>0</v>
       </c>
       <c r="AH3">
-        <v>0</v>
+        <v>0.00904238017927256</v>
       </c>
       <c r="AI3">
-        <v>0.008915787724415331</v>
+        <v>0.02444696682975859</v>
       </c>
       <c r="AJ3">
-        <v>0.02160668316878013</v>
+        <v>0.05629007326797934</v>
       </c>
     </row>
     <row r="4" spans="1:36">
@@ -897,55 +897,55 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>0.2847639121176406</v>
+        <v>0.1179134946918223</v>
       </c>
       <c r="F4">
-        <v>0.1407597575663971</v>
+        <v>0.0183554702629268</v>
       </c>
       <c r="G4">
-        <v>0.2709178435558056</v>
+        <v>0.09569603518254148</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>0.01209090311215746</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>0.07298728256956917</v>
       </c>
       <c r="J4">
-        <v>0</v>
+        <v>0.004563525169494958</v>
       </c>
       <c r="K4">
-        <v>0.1238003093150366</v>
+        <v>0</v>
       </c>
       <c r="L4">
-        <v>0.01895901933885585</v>
+        <v>0</v>
       </c>
       <c r="M4">
-        <v>0.03177633361973534</v>
+        <v>0.2620351786288969</v>
       </c>
       <c r="N4">
-        <v>0.004106824489686503</v>
+        <v>0.1249911123441372</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
       <c r="P4">
-        <v>0</v>
+        <v>0.06165712643233144</v>
       </c>
       <c r="Q4">
-        <v>0.003039826768261577</v>
+        <v>0</v>
       </c>
       <c r="R4">
-        <v>0</v>
+        <v>0.01252288916095265</v>
       </c>
       <c r="S4">
-        <v>0.01598442663664308</v>
+        <v>0</v>
       </c>
       <c r="T4">
         <v>0</v>
       </c>
       <c r="U4">
-        <v>0.004849594737302712</v>
+        <v>0.02995617729909208</v>
       </c>
       <c r="V4">
         <v>0</v>
@@ -954,10 +954,10 @@
         <v>0</v>
       </c>
       <c r="X4">
-        <v>0.06836687521874248</v>
+        <v>0.08403937075492668</v>
       </c>
       <c r="Y4">
-        <v>0</v>
+        <v>0.03347887952436204</v>
       </c>
       <c r="Z4">
         <v>0</v>
@@ -984,13 +984,13 @@
         <v>0</v>
       </c>
       <c r="AH4">
-        <v>0.000849403767639064</v>
+        <v>0</v>
       </c>
       <c r="AI4">
-        <v>0.01497005020782152</v>
+        <v>0.03039189379499306</v>
       </c>
       <c r="AJ4">
-        <v>0.01685582266043188</v>
+        <v>0.03932066107179593</v>
       </c>
     </row>
     <row r="5" spans="1:36">
@@ -1007,55 +1007,55 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>0.2016516135182773</v>
+        <v>0.1834483479035048</v>
       </c>
       <c r="F5">
-        <v>0.04034648798539808</v>
+        <v>0.09868925206733722</v>
       </c>
       <c r="G5">
-        <v>0.3233782875579669</v>
+        <v>0.1412585292806602</v>
       </c>
       <c r="H5">
-        <v>0.007408307741336323</v>
+        <v>0.05322447292395576</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>0.05325716232128996</v>
       </c>
       <c r="J5">
-        <v>0.03172615759207197</v>
+        <v>0</v>
       </c>
       <c r="K5">
-        <v>0.1075433285689083</v>
+        <v>0.02399020499160533</v>
       </c>
       <c r="L5">
-        <v>0.01045456113914201</v>
+        <v>0.01682131171582579</v>
       </c>
       <c r="M5">
-        <v>0.03323315708005286</v>
+        <v>0.1854228294438118</v>
       </c>
       <c r="N5">
-        <v>0.02547289721365328</v>
+        <v>0.003908067678128713</v>
       </c>
       <c r="O5">
         <v>0</v>
       </c>
       <c r="P5">
-        <v>0</v>
+        <v>0.07212393339297606</v>
       </c>
       <c r="Q5">
-        <v>0</v>
+        <v>0.02023687831029175</v>
       </c>
       <c r="R5">
-        <v>0.02467773573741563</v>
+        <v>0.0116978624894173</v>
       </c>
       <c r="S5">
-        <v>0.01150139106056939</v>
+        <v>0</v>
       </c>
       <c r="T5">
         <v>0</v>
       </c>
       <c r="U5">
-        <v>0.03517353274975801</v>
+        <v>0</v>
       </c>
       <c r="V5">
         <v>0</v>
@@ -1064,13 +1064,13 @@
         <v>0</v>
       </c>
       <c r="X5">
-        <v>0.09222974245457435</v>
+        <v>0.04340759332505884</v>
       </c>
       <c r="Y5">
-        <v>0.01130436783930669</v>
+        <v>0.02784244972854763</v>
       </c>
       <c r="Z5">
-        <v>0.02186882985574325</v>
+        <v>0</v>
       </c>
       <c r="AA5">
         <v>0</v>
@@ -1082,7 +1082,7 @@
         <v>0</v>
       </c>
       <c r="AD5">
-        <v>0</v>
+        <v>0.01068838288523369</v>
       </c>
       <c r="AE5">
         <v>0</v>
@@ -1091,16 +1091,16 @@
         <v>0</v>
       </c>
       <c r="AG5">
-        <v>0</v>
+        <v>0.003720983445460993</v>
       </c>
       <c r="AH5">
         <v>0</v>
       </c>
       <c r="AI5">
-        <v>0.003305170023756752</v>
+        <v>0.01395853284653089</v>
       </c>
       <c r="AJ5">
-        <v>0.01872443188206918</v>
+        <v>0.03630320525036314</v>
       </c>
     </row>
     <row r="6" spans="1:36">
@@ -1114,70 +1114,70 @@
         <v>0</v>
       </c>
       <c r="D6">
-        <v>0.005630125271338065</v>
+        <v>0</v>
       </c>
       <c r="E6">
-        <v>0.2212141198256587</v>
+        <v>0.1698418394585446</v>
       </c>
       <c r="F6">
-        <v>0.2265284776502698</v>
+        <v>0</v>
       </c>
       <c r="G6">
-        <v>0.1807452827802943</v>
+        <v>0.2449806199036375</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>0.08895842438740055</v>
       </c>
       <c r="I6">
         <v>0</v>
       </c>
       <c r="J6">
-        <v>0.005106432762393669</v>
+        <v>0.001065897181899224</v>
       </c>
       <c r="K6">
-        <v>0.1973088537913883</v>
+        <v>0.04107583087983967</v>
       </c>
       <c r="L6">
-        <v>0.01555486107933129</v>
+        <v>0.01856582489903747</v>
       </c>
       <c r="M6">
-        <v>0.003096913791262934</v>
+        <v>0.03782057311391854</v>
       </c>
       <c r="N6">
-        <v>0</v>
+        <v>0.08341615656435937</v>
       </c>
       <c r="O6">
         <v>0</v>
       </c>
       <c r="P6">
-        <v>0</v>
+        <v>0.009690195706483782</v>
       </c>
       <c r="Q6">
-        <v>0.009917407698003351</v>
+        <v>0</v>
       </c>
       <c r="R6">
-        <v>0</v>
+        <v>0.07012212624807908</v>
       </c>
       <c r="S6">
         <v>0</v>
       </c>
       <c r="T6">
-        <v>0.01354812936084224</v>
+        <v>0.01159324596035673</v>
       </c>
       <c r="U6">
-        <v>0</v>
+        <v>0.01929577644966685</v>
       </c>
       <c r="V6">
         <v>0</v>
       </c>
       <c r="W6">
-        <v>0.01871049013293005</v>
+        <v>0</v>
       </c>
       <c r="X6">
-        <v>0.0824615938098706</v>
+        <v>0.04538870475074969</v>
       </c>
       <c r="Y6">
-        <v>0</v>
+        <v>0.1042990517826987</v>
       </c>
       <c r="Z6">
         <v>0</v>
@@ -1204,13 +1204,13 @@
         <v>0</v>
       </c>
       <c r="AH6">
-        <v>0.002053884637459715</v>
+        <v>0</v>
       </c>
       <c r="AI6">
-        <v>0.01812342740895694</v>
+        <v>0.007503963675418255</v>
       </c>
       <c r="AJ6">
-        <v>0</v>
+        <v>0.04638176903791005</v>
       </c>
     </row>
   </sheetData>
@@ -1347,100 +1347,100 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>0.002056664043484111</v>
       </c>
       <c r="E2">
-        <v>0.1883562720413256</v>
+        <v>0.1313908317085751</v>
       </c>
       <c r="F2">
-        <v>0.2134614359331152</v>
+        <v>0.1521164865947558</v>
       </c>
       <c r="G2">
-        <v>0.4940755311239409</v>
+        <v>0.4276195501204607</v>
       </c>
       <c r="H2">
-        <v>0.4940755311239409</v>
+        <v>0.4937478051014808</v>
       </c>
       <c r="I2">
-        <v>0.4940755311239409</v>
+        <v>0.5141632497742766</v>
       </c>
       <c r="J2">
-        <v>0.5120718075705244</v>
+        <v>0.5141632497742766</v>
       </c>
       <c r="K2">
-        <v>0.6039596961801854</v>
+        <v>0.5141632497742766</v>
       </c>
       <c r="L2">
-        <v>0.6039596961801854</v>
+        <v>0.5141632497742766</v>
       </c>
       <c r="M2">
-        <v>0.6216893170214501</v>
+        <v>0.7547315322035367</v>
       </c>
       <c r="N2">
-        <v>0.7082050689098044</v>
+        <v>0.8021363251285796</v>
       </c>
       <c r="O2">
-        <v>0.71572069730995</v>
+        <v>0.8021363251285796</v>
       </c>
       <c r="P2">
-        <v>0.71572069730995</v>
+        <v>0.8608872393010963</v>
       </c>
       <c r="Q2">
-        <v>0.71572069730995</v>
+        <v>0.8707102250000635</v>
       </c>
       <c r="R2">
-        <v>0.7836422601120867</v>
+        <v>0.8905487418086843</v>
       </c>
       <c r="S2">
-        <v>0.792996967929276</v>
+        <v>0.9039457816448612</v>
       </c>
       <c r="T2">
-        <v>0.8024060459563362</v>
+        <v>0.9039457816448612</v>
       </c>
       <c r="U2">
-        <v>0.8649030417210005</v>
+        <v>0.9039457816448612</v>
       </c>
       <c r="V2">
-        <v>0.8649030417210005</v>
+        <v>0.9039457816448612</v>
       </c>
       <c r="W2">
-        <v>0.8658160515443823</v>
+        <v>0.9297602136609067</v>
       </c>
       <c r="X2">
-        <v>0.9512020154970848</v>
+        <v>0.9555036705530647</v>
       </c>
       <c r="Y2">
-        <v>0.9657133554803045</v>
+        <v>0.9658785843539063</v>
       </c>
       <c r="Z2">
-        <v>0.9861660468250008</v>
+        <v>0.9658785843539063</v>
       </c>
       <c r="AA2">
-        <v>0.9861660468250008</v>
+        <v>0.9658785843539063</v>
       </c>
       <c r="AB2">
-        <v>0.9861660468250008</v>
+        <v>0.9658785843539063</v>
       </c>
       <c r="AC2">
-        <v>0.9861660468250008</v>
+        <v>0.9658785843539063</v>
       </c>
       <c r="AD2">
-        <v>0.9861660468250008</v>
+        <v>0.9658785843539063</v>
       </c>
       <c r="AE2">
-        <v>0.9861660468250008</v>
+        <v>0.9658785843539063</v>
       </c>
       <c r="AF2">
-        <v>0.9861660468250008</v>
+        <v>0.9658785843539063</v>
       </c>
       <c r="AG2">
-        <v>0.9861660468250008</v>
+        <v>0.9658785843539063</v>
       </c>
       <c r="AH2">
-        <v>0.9861660468250008</v>
+        <v>0.9658785843539063</v>
       </c>
       <c r="AI2">
-        <v>0.9861660468250008</v>
+        <v>1</v>
       </c>
       <c r="AJ2">
         <v>1</v>
@@ -1460,97 +1460,97 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0.2810718858277978</v>
+        <v>0.1714552967088327</v>
       </c>
       <c r="F3">
-        <v>0.3767729848928042</v>
+        <v>0.1714552967088327</v>
       </c>
       <c r="G3">
-        <v>0.6849581931659249</v>
+        <v>0.2983263879009753</v>
       </c>
       <c r="H3">
-        <v>0.6849581931659249</v>
+        <v>0.4361606168251749</v>
       </c>
       <c r="I3">
-        <v>0.6849581931659249</v>
+        <v>0.5043991094398227</v>
       </c>
       <c r="J3">
-        <v>0.6892927023306435</v>
+        <v>0.5043991094398227</v>
       </c>
       <c r="K3">
-        <v>0.8040076679140001</v>
+        <v>0.5043991094398227</v>
       </c>
       <c r="L3">
-        <v>0.811943846677722</v>
+        <v>0.5043991094398227</v>
       </c>
       <c r="M3">
-        <v>0.83850035566433</v>
+        <v>0.6582496554550267</v>
       </c>
       <c r="N3">
-        <v>0.8503451259269302</v>
+        <v>0.6902915281852854</v>
       </c>
       <c r="O3">
-        <v>0.8503451259269302</v>
+        <v>0.6902915281852854</v>
       </c>
       <c r="P3">
-        <v>0.8503451259269302</v>
+        <v>0.7709127467378929</v>
       </c>
       <c r="Q3">
-        <v>0.8524707944528582</v>
+        <v>0.7709127467378929</v>
       </c>
       <c r="R3">
-        <v>0.8603999959865412</v>
+        <v>0.8375216342451512</v>
       </c>
       <c r="S3">
-        <v>0.8858791532281153</v>
+        <v>0.8375216342451512</v>
       </c>
       <c r="T3">
-        <v>0.8858791532281153</v>
+        <v>0.8375216342451512</v>
       </c>
       <c r="U3">
-        <v>0.9006076888876728</v>
+        <v>0.8459927518782109</v>
       </c>
       <c r="V3">
-        <v>0.9006076888876728</v>
+        <v>0.8459927518782109</v>
       </c>
       <c r="W3">
-        <v>0.9006076888876728</v>
+        <v>0.8536512569649255</v>
       </c>
       <c r="X3">
-        <v>0.9641103781698777</v>
+        <v>0.8784345126456055</v>
       </c>
       <c r="Y3">
-        <v>0.9641103781698777</v>
+        <v>0.8986173641455554</v>
       </c>
       <c r="Z3">
-        <v>0.9694775291068046</v>
+        <v>0.8986173641455554</v>
       </c>
       <c r="AA3">
-        <v>0.9694775291068046</v>
+        <v>0.8986173641455554</v>
       </c>
       <c r="AB3">
-        <v>0.9694775291068046</v>
+        <v>0.8986173641455554</v>
       </c>
       <c r="AC3">
-        <v>0.9694775291068046</v>
+        <v>0.8986173641455554</v>
       </c>
       <c r="AD3">
-        <v>0.9694775291068046</v>
+        <v>0.8986173641455554</v>
       </c>
       <c r="AE3">
-        <v>0.9694775291068046</v>
+        <v>0.9102205797229895</v>
       </c>
       <c r="AF3">
-        <v>0.9694775291068046</v>
+        <v>0.9102205797229895</v>
       </c>
       <c r="AG3">
-        <v>0.9694775291068046</v>
+        <v>0.9102205797229895</v>
       </c>
       <c r="AH3">
-        <v>0.9694775291068046</v>
+        <v>0.9192629599022621</v>
       </c>
       <c r="AI3">
-        <v>0.97839331683122</v>
+        <v>0.9437099267320207</v>
       </c>
       <c r="AJ3">
         <v>1</v>
@@ -1570,100 +1570,100 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>0.2847639121176406</v>
+        <v>0.1179134946918223</v>
       </c>
       <c r="F4">
-        <v>0.4255236696840377</v>
+        <v>0.1362689649547491</v>
       </c>
       <c r="G4">
-        <v>0.6964415132398433</v>
+        <v>0.2319650001372906</v>
       </c>
       <c r="H4">
-        <v>0.6964415132398433</v>
+        <v>0.2440559032494481</v>
       </c>
       <c r="I4">
-        <v>0.6964415132398433</v>
+        <v>0.3170431858190172</v>
       </c>
       <c r="J4">
-        <v>0.6964415132398433</v>
+        <v>0.3216067109885122</v>
       </c>
       <c r="K4">
-        <v>0.8202418225548799</v>
+        <v>0.3216067109885122</v>
       </c>
       <c r="L4">
-        <v>0.8392008418937358</v>
+        <v>0.3216067109885122</v>
       </c>
       <c r="M4">
-        <v>0.8709771755134711</v>
+        <v>0.5836418896174091</v>
       </c>
       <c r="N4">
-        <v>0.8750840000031576</v>
+        <v>0.7086330019615463</v>
       </c>
       <c r="O4">
-        <v>0.8750840000031576</v>
+        <v>0.7086330019615463</v>
       </c>
       <c r="P4">
-        <v>0.8750840000031576</v>
+        <v>0.7702901283938778</v>
       </c>
       <c r="Q4">
-        <v>0.8781238267714191</v>
+        <v>0.7702901283938778</v>
       </c>
       <c r="R4">
-        <v>0.8781238267714191</v>
+        <v>0.7828130175548305</v>
       </c>
       <c r="S4">
-        <v>0.8941082534080622</v>
+        <v>0.7828130175548305</v>
       </c>
       <c r="T4">
-        <v>0.8941082534080622</v>
+        <v>0.7828130175548305</v>
       </c>
       <c r="U4">
-        <v>0.8989578481453649</v>
+        <v>0.8127691948539225</v>
       </c>
       <c r="V4">
-        <v>0.8989578481453649</v>
+        <v>0.8127691948539225</v>
       </c>
       <c r="W4">
-        <v>0.8989578481453649</v>
+        <v>0.8127691948539225</v>
       </c>
       <c r="X4">
-        <v>0.9673247233641075</v>
+        <v>0.8968085656088491</v>
       </c>
       <c r="Y4">
-        <v>0.9673247233641075</v>
+        <v>0.9302874451332112</v>
       </c>
       <c r="Z4">
-        <v>0.9673247233641075</v>
+        <v>0.9302874451332112</v>
       </c>
       <c r="AA4">
-        <v>0.9673247233641075</v>
+        <v>0.9302874451332112</v>
       </c>
       <c r="AB4">
-        <v>0.9673247233641075</v>
+        <v>0.9302874451332112</v>
       </c>
       <c r="AC4">
-        <v>0.9673247233641075</v>
+        <v>0.9302874451332112</v>
       </c>
       <c r="AD4">
-        <v>0.9673247233641075</v>
+        <v>0.9302874451332112</v>
       </c>
       <c r="AE4">
-        <v>0.9673247233641075</v>
+        <v>0.9302874451332112</v>
       </c>
       <c r="AF4">
-        <v>0.9673247233641075</v>
+        <v>0.9302874451332112</v>
       </c>
       <c r="AG4">
-        <v>0.9673247233641075</v>
+        <v>0.9302874451332112</v>
       </c>
       <c r="AH4">
-        <v>0.9681741271317466</v>
+        <v>0.9302874451332112</v>
       </c>
       <c r="AI4">
-        <v>0.983144177339568</v>
+        <v>0.9606793389282042</v>
       </c>
       <c r="AJ4">
-        <v>0.9999999999999999</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:36">
@@ -1680,100 +1680,100 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>0.2016516135182773</v>
+        <v>0.1834483479035048</v>
       </c>
       <c r="F5">
-        <v>0.2419981015036753</v>
+        <v>0.282137599970842</v>
       </c>
       <c r="G5">
-        <v>0.5653763890616422</v>
+        <v>0.4233961292515022</v>
       </c>
       <c r="H5">
-        <v>0.5727846968029785</v>
+        <v>0.4766206021754579</v>
       </c>
       <c r="I5">
-        <v>0.5727846968029785</v>
+        <v>0.5298777644967478</v>
       </c>
       <c r="J5">
-        <v>0.6045108543950505</v>
+        <v>0.5298777644967478</v>
       </c>
       <c r="K5">
-        <v>0.7120541829639587</v>
+        <v>0.5538679694883532</v>
       </c>
       <c r="L5">
-        <v>0.7225087441031007</v>
+        <v>0.5706892812041789</v>
       </c>
       <c r="M5">
-        <v>0.7557419011831535</v>
+        <v>0.7561121106479907</v>
       </c>
       <c r="N5">
-        <v>0.7812147983968069</v>
+        <v>0.7600201783261193</v>
       </c>
       <c r="O5">
-        <v>0.7812147983968069</v>
+        <v>0.7600201783261193</v>
       </c>
       <c r="P5">
-        <v>0.7812147983968069</v>
+        <v>0.8321441117190954</v>
       </c>
       <c r="Q5">
-        <v>0.7812147983968069</v>
+        <v>0.8523809900293872</v>
       </c>
       <c r="R5">
-        <v>0.8058925341342225</v>
+        <v>0.8640788525188045</v>
       </c>
       <c r="S5">
-        <v>0.8173939251947918</v>
+        <v>0.8640788525188045</v>
       </c>
       <c r="T5">
-        <v>0.8173939251947918</v>
+        <v>0.8640788525188045</v>
       </c>
       <c r="U5">
-        <v>0.8525674579445498</v>
+        <v>0.8640788525188045</v>
       </c>
       <c r="V5">
-        <v>0.8525674579445498</v>
+        <v>0.8640788525188045</v>
       </c>
       <c r="W5">
-        <v>0.8525674579445498</v>
+        <v>0.8640788525188045</v>
       </c>
       <c r="X5">
-        <v>0.9447972003991242</v>
+        <v>0.9074864458438633</v>
       </c>
       <c r="Y5">
-        <v>0.9561015682384308</v>
+        <v>0.9353288955724109</v>
       </c>
       <c r="Z5">
-        <v>0.9779703980941741</v>
+        <v>0.9353288955724109</v>
       </c>
       <c r="AA5">
-        <v>0.9779703980941741</v>
+        <v>0.9353288955724109</v>
       </c>
       <c r="AB5">
-        <v>0.9779703980941741</v>
+        <v>0.9353288955724109</v>
       </c>
       <c r="AC5">
-        <v>0.9779703980941741</v>
+        <v>0.9353288955724109</v>
       </c>
       <c r="AD5">
-        <v>0.9779703980941741</v>
+        <v>0.9460172784576446</v>
       </c>
       <c r="AE5">
-        <v>0.9779703980941741</v>
+        <v>0.9460172784576446</v>
       </c>
       <c r="AF5">
-        <v>0.9779703980941741</v>
+        <v>0.9460172784576446</v>
       </c>
       <c r="AG5">
-        <v>0.9779703980941741</v>
+        <v>0.9497382619031056</v>
       </c>
       <c r="AH5">
-        <v>0.9779703980941741</v>
+        <v>0.9497382619031056</v>
       </c>
       <c r="AI5">
-        <v>0.9812755681179308</v>
+        <v>0.9636967947496365</v>
       </c>
       <c r="AJ5">
-        <v>1</v>
+        <v>0.9999999999999997</v>
       </c>
     </row>
     <row r="6" spans="1:36">
@@ -1787,103 +1787,103 @@
         <v>0</v>
       </c>
       <c r="D6">
-        <v>0.005630125271338065</v>
+        <v>0</v>
       </c>
       <c r="E6">
-        <v>0.2268442450969968</v>
+        <v>0.1698418394585446</v>
       </c>
       <c r="F6">
-        <v>0.4533727227472666</v>
+        <v>0.1698418394585446</v>
       </c>
       <c r="G6">
-        <v>0.6341180055275609</v>
+        <v>0.4148224593621821</v>
       </c>
       <c r="H6">
-        <v>0.6341180055275609</v>
+        <v>0.5037808837495826</v>
       </c>
       <c r="I6">
-        <v>0.6341180055275609</v>
+        <v>0.5037808837495826</v>
       </c>
       <c r="J6">
-        <v>0.6392244382899546</v>
+        <v>0.5048467809314818</v>
       </c>
       <c r="K6">
-        <v>0.8365332920813429</v>
+        <v>0.5459226118113215</v>
       </c>
       <c r="L6">
-        <v>0.8520881531606741</v>
+        <v>0.564488436710359</v>
       </c>
       <c r="M6">
-        <v>0.8551850669519371</v>
+        <v>0.6023090098242775</v>
       </c>
       <c r="N6">
-        <v>0.8551850669519371</v>
+        <v>0.6857251663886369</v>
       </c>
       <c r="O6">
-        <v>0.8551850669519371</v>
+        <v>0.6857251663886369</v>
       </c>
       <c r="P6">
-        <v>0.8551850669519371</v>
+        <v>0.6954153620951207</v>
       </c>
       <c r="Q6">
-        <v>0.8651024746499404</v>
+        <v>0.6954153620951207</v>
       </c>
       <c r="R6">
-        <v>0.8651024746499404</v>
+        <v>0.7655374883431998</v>
       </c>
       <c r="S6">
-        <v>0.8651024746499404</v>
+        <v>0.7655374883431998</v>
       </c>
       <c r="T6">
-        <v>0.8786506040107827</v>
+        <v>0.7771307343035565</v>
       </c>
       <c r="U6">
-        <v>0.8786506040107827</v>
+        <v>0.7964265107532233</v>
       </c>
       <c r="V6">
-        <v>0.8786506040107827</v>
+        <v>0.7964265107532233</v>
       </c>
       <c r="W6">
-        <v>0.8973610941437127</v>
+        <v>0.7964265107532233</v>
       </c>
       <c r="X6">
-        <v>0.9798226879535833</v>
+        <v>0.8418152155039731</v>
       </c>
       <c r="Y6">
-        <v>0.9798226879535833</v>
+        <v>0.9461142672866718</v>
       </c>
       <c r="Z6">
-        <v>0.9798226879535833</v>
+        <v>0.9461142672866718</v>
       </c>
       <c r="AA6">
-        <v>0.9798226879535833</v>
+        <v>0.9461142672866718</v>
       </c>
       <c r="AB6">
-        <v>0.9798226879535833</v>
+        <v>0.9461142672866718</v>
       </c>
       <c r="AC6">
-        <v>0.9798226879535833</v>
+        <v>0.9461142672866718</v>
       </c>
       <c r="AD6">
-        <v>0.9798226879535833</v>
+        <v>0.9461142672866718</v>
       </c>
       <c r="AE6">
-        <v>0.9798226879535833</v>
+        <v>0.9461142672866718</v>
       </c>
       <c r="AF6">
-        <v>0.9798226879535833</v>
+        <v>0.9461142672866718</v>
       </c>
       <c r="AG6">
-        <v>0.9798226879535833</v>
+        <v>0.9461142672866718</v>
       </c>
       <c r="AH6">
-        <v>0.981876572591043</v>
+        <v>0.9461142672866718</v>
       </c>
       <c r="AI6">
-        <v>0.9999999999999999</v>
+        <v>0.9536182309620901</v>
       </c>
       <c r="AJ6">
-        <v>0.9999999999999999</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1951,16 +1951,16 @@
         <v>2</v>
       </c>
       <c r="D2">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>0.5120718075705244</v>
+        <v>0.5141632497742766</v>
       </c>
       <c r="G2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H2">
         <v>10</v>
@@ -1992,16 +1992,16 @@
         <v>2</v>
       </c>
       <c r="D3">
+        <v>8</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0.5043991094398227</v>
+      </c>
+      <c r="G3">
         <v>6</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0.6849581931659249</v>
-      </c>
-      <c r="G3">
-        <v>4</v>
       </c>
       <c r="H3">
         <v>10</v>
@@ -2033,16 +2033,16 @@
         <v>2</v>
       </c>
       <c r="D4">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4">
-        <v>0.6964415132398433</v>
+        <v>0.5836418896174091</v>
       </c>
       <c r="G4">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="H4">
         <v>10</v>
@@ -2074,16 +2074,16 @@
         <v>2</v>
       </c>
       <c r="D5">
+        <v>8</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0.5298777644967478</v>
+      </c>
+      <c r="G5">
         <v>6</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>0.5653763890616422</v>
-      </c>
-      <c r="G5">
-        <v>4</v>
       </c>
       <c r="H5">
         <v>10</v>
@@ -2115,16 +2115,16 @@
         <v>2</v>
       </c>
       <c r="D6">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6">
-        <v>0.6341180055275609</v>
+        <v>0.5037808837495826</v>
       </c>
       <c r="G6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H6">
         <v>10</v>
@@ -2210,16 +2210,16 @@
         <v>2</v>
       </c>
       <c r="D2">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>0.7082050689098044</v>
+        <v>0.7547315322035367</v>
       </c>
       <c r="G2">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H2">
         <v>10</v>
@@ -2251,16 +2251,16 @@
         <v>2</v>
       </c>
       <c r="D3">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3">
-        <v>0.8040076679140001</v>
+        <v>0.7709127467378929</v>
       </c>
       <c r="G3">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="H3">
         <v>10</v>
@@ -2292,16 +2292,16 @@
         <v>2</v>
       </c>
       <c r="D4">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4">
-        <v>0.8202418225548799</v>
+        <v>0.7086330019615463</v>
       </c>
       <c r="G4">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="H4">
         <v>10</v>
@@ -2333,16 +2333,16 @@
         <v>2</v>
       </c>
       <c r="D5">
+        <v>12</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0.7561121106479907</v>
+      </c>
+      <c r="G5">
         <v>10</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>0.7120541829639587</v>
-      </c>
-      <c r="G5">
-        <v>8</v>
       </c>
       <c r="H5">
         <v>10</v>
@@ -2374,16 +2374,16 @@
         <v>2</v>
       </c>
       <c r="D6">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6">
-        <v>0.8365332920813429</v>
+        <v>0.7655374883431998</v>
       </c>
       <c r="G6">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="H6">
         <v>10</v>
@@ -2469,16 +2469,16 @@
         <v>2</v>
       </c>
       <c r="D2">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>0.8024060459563362</v>
+        <v>0.8021363251285796</v>
       </c>
       <c r="G2">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="H2">
         <v>10</v>
@@ -2510,16 +2510,16 @@
         <v>2</v>
       </c>
       <c r="D3">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3">
-        <v>0.8040076679140001</v>
+        <v>0.8375216342451512</v>
       </c>
       <c r="G3">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="H3">
         <v>10</v>
@@ -2551,16 +2551,16 @@
         <v>2</v>
       </c>
       <c r="D4">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4">
-        <v>0.8202418225548799</v>
+        <v>0.8127691948539225</v>
       </c>
       <c r="G4">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="H4">
         <v>10</v>
@@ -2592,16 +2592,16 @@
         <v>2</v>
       </c>
       <c r="D5">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5">
-        <v>0.8058925341342225</v>
+        <v>0.8321441117190954</v>
       </c>
       <c r="G5">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H5">
         <v>10</v>
@@ -2633,16 +2633,16 @@
         <v>2</v>
       </c>
       <c r="D6">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6">
-        <v>0.8365332920813429</v>
+        <v>0.8418152155039731</v>
       </c>
       <c r="G6">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="H6">
         <v>10</v>
@@ -2728,16 +2728,16 @@
         <v>2</v>
       </c>
       <c r="D2">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>0.9512020154970848</v>
+        <v>0.9039457816448612</v>
       </c>
       <c r="G2">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="H2">
         <v>10</v>
@@ -2769,16 +2769,16 @@
         <v>2</v>
       </c>
       <c r="D3">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3">
-        <v>0.9006076888876728</v>
+        <v>0.9102205797229895</v>
       </c>
       <c r="G3">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="H3">
         <v>10</v>
@@ -2810,16 +2810,16 @@
         <v>2</v>
       </c>
       <c r="D4">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4">
-        <v>0.9673247233641075</v>
+        <v>0.9302874451332112</v>
       </c>
       <c r="G4">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H4">
         <v>10</v>
@@ -2857,7 +2857,7 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>0.9447972003991242</v>
+        <v>0.9074864458438633</v>
       </c>
       <c r="G5">
         <v>21</v>
@@ -2892,16 +2892,16 @@
         <v>2</v>
       </c>
       <c r="D6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6">
-        <v>0.9798226879535833</v>
+        <v>0.9461142672866718</v>
       </c>
       <c r="G6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H6">
         <v>10</v>

</xml_diff>